<commit_message>
added writing document. Made general edits... switched names accidentally
</commit_message>
<xml_diff>
--- a/2.Excel/test.xlsx
+++ b/2.Excel/test.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="64" documentId="8_{05EC9499-347C-4F33-8DCF-A8355338C733}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A39D319-DF25-483D-BB3C-8E599987DEBA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0FEADDDF-684B-4A90-A003-AF417A99AAAA}"/>
+    <workbookView xWindow="14220" yWindow="5115" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{0FEADDDF-684B-4A90-A003-AF417A99AAAA}"/>
   </bookViews>
   <sheets>
     <sheet name="MySheet" sheetId="1" r:id="rId1"/>
@@ -521,7 +521,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>